<commit_message>
cho thuê xe, tiền trừ dần vào tài khoản
</commit_message>
<xml_diff>
--- a/Bicycle-Rental/asset/History.xlsx
+++ b/Bicycle-Rental/asset/History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Temp\Bicycle-Rental\Bicycle-Rental\asset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8C8B26-0436-4E45-8ED5-4078FD710728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782EEC33-9719-4B0D-BC89-10B741CDAD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>loaixe</t>
+  </si>
+  <si>
+    <t>thanhtoan</t>
   </si>
 </sst>
 </file>
@@ -360,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,16 +379,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>